<commit_message>
Fixed bug where second session would crash. Misc fixes . also added preference for having network location or not.
</commit_message>
<xml_diff>
--- a/Analysis/server0s5p/client0.1s/csr600d0.1v2.xlsx
+++ b/Analysis/server0s5p/client0.1s/csr600d0.1v2.xlsx
@@ -10917,11 +10917,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107469440"/>
-        <c:axId val="120037760"/>
+        <c:axId val="101223808"/>
+        <c:axId val="101237888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107469440"/>
+        <c:axId val="101223808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10931,7 +10931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120037760"/>
+        <c:crossAx val="101237888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10939,7 +10939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120037760"/>
+        <c:axId val="101237888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10950,7 +10950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107469440"/>
+        <c:crossAx val="101223808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11298,8 +11298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:LT104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="O103" sqref="O103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27998,7 +27998,7 @@
         <v>1004</v>
       </c>
       <c r="LO83">
-        <f t="shared" ref="LO83:NZ83" si="6">LO18-LN18</f>
+        <f t="shared" ref="LO83:LS83" si="6">LO18-LN18</f>
         <v>1003</v>
       </c>
       <c r="LP83">
@@ -29323,7 +29323,7 @@
         <v>1035</v>
       </c>
       <c r="LO84">
-        <f t="shared" ref="LO84:NZ84" si="13">LO45-LN45</f>
+        <f t="shared" ref="LO84:LS84" si="13">LO45-LN45</f>
         <v>1017</v>
       </c>
       <c r="LP84">
@@ -30648,7 +30648,7 @@
         <v>1019</v>
       </c>
       <c r="LO85">
-        <f t="shared" ref="LO85:NZ85" si="20">LO72-LN72</f>
+        <f t="shared" ref="LO85:LS85" si="20">LO72-LN72</f>
         <v>1015</v>
       </c>
       <c r="LP85">
@@ -32776,7 +32776,7 @@
         <v>-320</v>
       </c>
       <c r="JQ88">
-        <f t="shared" ref="JQ88:MB88" si="27">JP47-JP18</f>
+        <f t="shared" ref="JQ88:LT88" si="27">JP47-JP18</f>
         <v>-308</v>
       </c>
       <c r="JR88">
@@ -34105,7 +34105,7 @@
         <v>-315</v>
       </c>
       <c r="JQ89">
-        <f t="shared" ref="JQ89:MB89" si="34">JP74-JP18</f>
+        <f t="shared" ref="JQ89:LT89" si="34">JP74-JP18</f>
         <v>-302</v>
       </c>
       <c r="JR89">
@@ -35434,7 +35434,7 @@
         <v>129462</v>
       </c>
       <c r="JQ90">
-        <f t="shared" ref="JQ90:MB90" si="41">JP22-JP45</f>
+        <f t="shared" ref="JQ90:LT90" si="41">JP22-JP45</f>
         <v>128451</v>
       </c>
       <c r="JR90">
@@ -36763,7 +36763,7 @@
         <v>21528</v>
       </c>
       <c r="JQ91">
-        <f t="shared" ref="JQ91:MB91" si="48">JP76-JP45</f>
+        <f t="shared" ref="JQ91:LT91" si="48">JP76-JP45</f>
         <v>394</v>
       </c>
       <c r="JR91">
@@ -38092,7 +38092,7 @@
         <v>238672</v>
       </c>
       <c r="JQ92">
-        <f t="shared" ref="JQ92:MB92" si="55">JP24-JP72</f>
+        <f t="shared" ref="JQ92:LT92" si="55">JP24-JP72</f>
         <v>237662</v>
       </c>
       <c r="JR92">
@@ -39421,7 +39421,7 @@
         <v>-6</v>
       </c>
       <c r="JQ93">
-        <f t="shared" ref="JQ93:MB93" si="62">JP51-JP72</f>
+        <f t="shared" ref="JQ93:LT93" si="62">JP51-JP72</f>
         <v>-12</v>
       </c>
       <c r="JR93">
@@ -41741,7 +41741,7 @@
         <v>331</v>
       </c>
       <c r="KJ97">
-        <f t="shared" ref="KJ97:KW97" si="72">FREQUENCY($B88:$QY88, KJ$96)</f>
+        <f t="shared" ref="KJ97:KT97" si="72">FREQUENCY($B88:$QY88, KJ$96)</f>
         <v>331</v>
       </c>
       <c r="KK97">
@@ -42962,7 +42962,7 @@
         <v>331</v>
       </c>
       <c r="KJ98">
-        <f t="shared" ref="KJ98:KW98" si="81">FREQUENCY($B89:$QY89, KJ$96)</f>
+        <f t="shared" ref="KJ98:KT98" si="81">FREQUENCY($B89:$QY89, KJ$96)</f>
         <v>331</v>
       </c>
       <c r="KK98">
@@ -44183,7 +44183,7 @@
         <v>331</v>
       </c>
       <c r="KJ99">
-        <f t="shared" ref="KJ99:KW99" si="89">FREQUENCY($B90:$QY90, KJ$96)</f>
+        <f t="shared" ref="KJ99:KT99" si="89">FREQUENCY($B90:$QY90, KJ$96)</f>
         <v>331</v>
       </c>
       <c r="KK99">
@@ -45404,7 +45404,7 @@
         <v>331</v>
       </c>
       <c r="KJ100">
-        <f t="shared" ref="KJ100:KW100" si="97">FREQUENCY($B91:$QY91, KJ$96)</f>
+        <f t="shared" ref="KJ100:KT100" si="97">FREQUENCY($B91:$QY91, KJ$96)</f>
         <v>331</v>
       </c>
       <c r="KK100">
@@ -46625,7 +46625,7 @@
         <v>320</v>
       </c>
       <c r="KJ101">
-        <f t="shared" ref="KJ101:KW101" si="105">FREQUENCY($B92:$QY92, KJ$96)</f>
+        <f t="shared" ref="KJ101:KT101" si="105">FREQUENCY($B92:$QY92, KJ$96)</f>
         <v>321</v>
       </c>
       <c r="KK101">
@@ -47846,7 +47846,7 @@
         <v>331</v>
       </c>
       <c r="KJ102">
-        <f t="shared" ref="KJ102:KW102" si="113">FREQUENCY($B93:$QY93, KJ$96)</f>
+        <f t="shared" ref="KJ102:KT102" si="113">FREQUENCY($B93:$QY93, KJ$96)</f>
         <v>331</v>
       </c>
       <c r="KK102">

</xml_diff>